<commit_message>
Fixing BOM. Wrong samtec connector was omitted !!!!!
</commit_message>
<xml_diff>
--- a/meta/src/meta_module_bom_rev1.xlsx
+++ b/meta/src/meta_module_bom_rev1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -133,12 +133,6 @@
     <t>CONN RCPT 240POS 0.5MM SMD</t>
   </si>
   <si>
-    <t>J18</t>
-  </si>
-  <si>
-    <t>J1,J3,J5,J6,J16</t>
-  </si>
-  <si>
     <t>col0-pu</t>
   </si>
   <si>
@@ -270,6 +264,12 @@
   </si>
   <si>
     <t>Capacitor 100uF 6.3V X5R 20% LOW ESR 1210</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>J1,J3,J5,J6,J18</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1186,7 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1245,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -1294,7 +1294,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -1367,7 +1367,7 @@
         <v>256</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>26</v>
@@ -1412,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>23</v>
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>36</v>
@@ -1485,36 +1485,36 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="7">
         <v>164</v>
@@ -1541,12 +1541,12 @@
         <v>171</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4">
         <v>50</v>
@@ -1573,12 +1573,12 @@
         <v>57</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7">
         <v>392</v>
@@ -1605,12 +1605,12 @@
         <v>399</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4">
         <v>278</v>
@@ -1637,12 +1637,12 @@
         <v>285</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7">
         <v>221</v>
@@ -1669,12 +1669,12 @@
         <v>228</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="4">
         <v>107</v>
@@ -1701,12 +1701,12 @@
         <v>114</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="7">
         <v>449</v>
@@ -1733,12 +1733,12 @@
         <v>456</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4">
         <v>335</v>
@@ -1765,12 +1765,12 @@
         <v>342</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7">
         <v>620</v>
@@ -1797,12 +1797,12 @@
         <v>627</v>
       </c>
       <c r="K10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="4">
         <v>506</v>
@@ -1829,12 +1829,12 @@
         <v>513</v>
       </c>
       <c r="K11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="7">
         <v>848</v>
@@ -1861,12 +1861,12 @@
         <v>855</v>
       </c>
       <c r="K12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="4">
         <v>734</v>
@@ -1893,12 +1893,12 @@
         <v>741</v>
       </c>
       <c r="K13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7">
         <v>677</v>
@@ -1925,12 +1925,12 @@
         <v>684</v>
       </c>
       <c r="K14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="4">
         <v>563</v>
@@ -1957,12 +1957,12 @@
         <v>570</v>
       </c>
       <c r="K15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="7">
         <v>905</v>
@@ -1989,12 +1989,12 @@
         <v>912</v>
       </c>
       <c r="K16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="4">
         <v>791</v>
@@ -2021,7 +2021,7 @@
         <v>798</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>